<commit_message>
update them report thong ke doanh thu
</commit_message>
<xml_diff>
--- a/Do An Quan Ly Nha Hang/DoAnQuanLyNhaHang/DoAnQuanLyNhaHang/bin/Debug/HoaDon.xlsx
+++ b/Do An Quan Ly Nha Hang/DoAnQuanLyNhaHang/DoAnQuanLyNhaHang/bin/Debug/HoaDon.xlsx
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>